<commit_message>
add leitura de base e criação do arquivo de saída
</commit_message>
<xml_diff>
--- a/Arquivos/BaseA.xlsx
+++ b/Arquivos/BaseA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jairm\Documents\Code\Empilhador\Arquivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jairm\Documents\Code\Empilhador\empilhador\Arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -350,8 +350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Correção do erro que só empilhava os dois primeiros campos
</commit_message>
<xml_diff>
--- a/Arquivos/BaseA.xlsx
+++ b/Arquivos/BaseA.xlsx
@@ -24,12 +24,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Nome</t>
   </si>
   <si>
-    <t>Data</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>VALOR</t>
+  </si>
+  <si>
+    <t>NOME_1</t>
+  </si>
+  <si>
+    <t>NOME_2</t>
+  </si>
+  <si>
+    <t>NOME_3</t>
+  </si>
+  <si>
+    <t>NOME_4</t>
+  </si>
+  <si>
+    <t>NOME_5</t>
+  </si>
+  <si>
+    <t>NOME_6</t>
+  </si>
+  <si>
+    <t>NOME_7</t>
+  </si>
+  <si>
+    <t>NOME_8</t>
+  </si>
+  <si>
+    <t>NOME_9</t>
+  </si>
+  <si>
+    <t>NOME_10</t>
+  </si>
+  <si>
+    <t>NOME_11</t>
+  </si>
+  <si>
+    <t>NOME_12</t>
+  </si>
+  <si>
+    <t>NOME_13</t>
+  </si>
+  <si>
+    <t>NOME_14</t>
+  </si>
+  <si>
+    <t>NOME_15</t>
   </si>
 </sst>
 </file>
@@ -67,7 +115,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -359,132 +407,180 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43709</v>
-      </c>
-      <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43710</v>
-      </c>
-      <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>43711</v>
-      </c>
-      <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43712</v>
-      </c>
-      <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>43713</v>
-      </c>
-      <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43714</v>
-      </c>
-      <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43715</v>
-      </c>
-      <c r="B8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43716</v>
-      </c>
-      <c r="B9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43717</v>
-      </c>
-      <c r="B10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43718</v>
-      </c>
-      <c r="B11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43719</v>
-      </c>
-      <c r="B12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>43720</v>
-      </c>
-      <c r="B13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>43721</v>
-      </c>
-      <c r="B14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>43722</v>
-      </c>
-      <c r="B15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>43723</v>
-      </c>
-      <c r="B16">
         <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização base e arquivo config
</commit_message>
<xml_diff>
--- a/Arquivos/BaseA.xlsx
+++ b/Arquivos/BaseA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nome</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>NOME_15</t>
+  </si>
+  <si>
+    <t>ID2</t>
   </si>
 </sst>
 </file>
@@ -396,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C16"/>
+      <selection activeCell="D2" sqref="D2:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +410,7 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -417,8 +420,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -428,8 +434,11 @@
       <c r="C2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -439,8 +448,11 @@
       <c r="C3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -450,8 +462,11 @@
       <c r="C4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -461,8 +476,11 @@
       <c r="C5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -472,8 +490,11 @@
       <c r="C6">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -483,8 +504,11 @@
       <c r="C7">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -494,8 +518,11 @@
       <c r="C8">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -505,8 +532,11 @@
       <c r="C9">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -516,8 +546,11 @@
       <c r="C10">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -527,8 +560,11 @@
       <c r="C11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -538,8 +574,11 @@
       <c r="C12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -549,8 +588,11 @@
       <c r="C13">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -560,8 +602,11 @@
       <c r="C14">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -571,8 +616,11 @@
       <c r="C15">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -581,6 +629,9 @@
       </c>
       <c r="C16">
         <v>51</v>
+      </c>
+      <c r="D16">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>